<commit_message>
Added unit testing for SimpleGame.NewTurn and GeneralGame.NewTurn
</commit_message>
<xml_diff>
--- a/artifacts/sprint-2-logs.xlsx
+++ b/artifacts/sprint-2-logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d987dc1895f9fb9d/School/SoftwareFoundations/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbens\dev\sosgame\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2518" documentId="11_F25DC773A252ABDACC1048B6515D41CC5ADE58FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E59F3ED-87F1-45CC-9140-F35EC69F1E8B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F837AB4F-3B23-4883-9BC2-C96A0D10631A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="16410" windowHeight="11295" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Summary of Source Code" sheetId="4" r:id="rId3"/>
     <sheet name="Production Code" sheetId="5" r:id="rId4"/>
     <sheet name="Automated Test Code" sheetId="6" r:id="rId5"/>
-    <sheet name="Manual Test Code" sheetId="10" r:id="rId6"/>
+    <sheet name="Manual Tests" sheetId="10" r:id="rId6"/>
     <sheet name="Additional Automated Tests" sheetId="11" r:id="rId7"/>
     <sheet name="Accessibility Table" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -1180,12 +1180,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1195,11 +1189,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="62">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1279,15 +1321,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1303,46 +1336,13 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1450,83 +1450,83 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}" name="Table5" displayName="Table5" ref="B4:I23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}" name="Table5" displayName="Table5" ref="B4:I23" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="B4:I23" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{FA37DF55-838D-4C91-A069-B4ADFBB114FF}" name="Story ID" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{B29593B2-9E50-4429-B73E-C267894CE53F}" name="Story Name" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{92144E97-78C1-4013-A5DC-A103AC987D08}" name="AC  ID" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{D34169B1-9605-4002-A5FC-55DBEC95591D}" name="AC Name" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{988A7BC5-9B7F-4EF4-9743-8B43044CA88C}" name="Classes" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{6962998B-BD75-44D2-8DE4-A3B7232E7D55}" name="Method Name(s) " dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{8D2432C4-71E4-445C-BF93-B65E87280890}" name="Status" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{1E10CD18-6EE0-4C57-A597-745A6F075070}" name="Notes (optional)" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{FA37DF55-838D-4C91-A069-B4ADFBB114FF}" name="Story ID" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{B29593B2-9E50-4429-B73E-C267894CE53F}" name="Story Name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{92144E97-78C1-4013-A5DC-A103AC987D08}" name="AC  ID" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{D34169B1-9605-4002-A5FC-55DBEC95591D}" name="AC Name" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{988A7BC5-9B7F-4EF4-9743-8B43044CA88C}" name="Classes" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{6962998B-BD75-44D2-8DE4-A3B7232E7D55}" name="Method Name(s) " dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{8D2432C4-71E4-445C-BF93-B65E87280890}" name="Status" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{1E10CD18-6EE0-4C57-A597-745A6F075070}" name="Notes (optional)" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}" name="Table6" displayName="Table6" ref="B3:H24" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}" name="Table6" displayName="Table6" ref="B3:H24" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="B3:H24" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4D464094-4CAA-4F0A-8155-1005A5221EA7}" name="User Story ID" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{DFFD886B-21F5-4EE4-B1E5-B9C3CA981393}" name="User Story Name" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{588A5FF9-87E4-4232-A109-F00AE6EAB7C9}" name="AC ID" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{A723F0C9-F396-4182-A5DB-A36687ECC464}" name="AC Name" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{04A7B299-94AB-4FB7-8A08-822F463E676E}" name="Classes " dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{263669AA-535C-4DA8-9C9A-A153A480F553}" name="Methods" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{9CFC3D83-A897-493C-A6B2-E4D0BA51E596}" name="Description" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{4D464094-4CAA-4F0A-8155-1005A5221EA7}" name="User Story ID" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{DFFD886B-21F5-4EE4-B1E5-B9C3CA981393}" name="User Story Name" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{588A5FF9-87E4-4232-A109-F00AE6EAB7C9}" name="AC ID" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{A723F0C9-F396-4182-A5DB-A36687ECC464}" name="AC Name" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{04A7B299-94AB-4FB7-8A08-822F463E676E}" name="Classes " dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{263669AA-535C-4DA8-9C9A-A153A480F553}" name="Methods" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{9CFC3D83-A897-493C-A6B2-E4D0BA51E596}" name="Description" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A6E1AD56-1E7E-4845-A6DC-51274101CF0C}" name="Table69" displayName="Table69" ref="B3:G19" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A6E1AD56-1E7E-4845-A6DC-51274101CF0C}" name="Table69" displayName="Table69" ref="B3:G19" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="B3:G19" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{301EF044-7DF2-4C9B-84A0-556EDC81E926}" name="User Story ID" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{C53176BB-A112-4BC9-B43C-A9B819FD40BE}" name="User Story Name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{75701814-A8A2-49F2-9634-F7BCE794B67D}" name="AC ID" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{DB2FE0C2-4D4A-4FA4-AD4F-2F9ACE0E2772}" name="AC Name" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{5FE8A6D0-B4D1-471F-9956-459A848C1C0F}" name="Test Case Input" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{C8A349CF-C07B-44C4-B8D0-DD604B478305}" name="Test Oracle" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{301EF044-7DF2-4C9B-84A0-556EDC81E926}" name="User Story ID" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C53176BB-A112-4BC9-B43C-A9B819FD40BE}" name="User Story Name" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{75701814-A8A2-49F2-9634-F7BCE794B67D}" name="AC ID" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{DB2FE0C2-4D4A-4FA4-AD4F-2F9ACE0E2772}" name="AC Name" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{5FE8A6D0-B4D1-471F-9956-459A848C1C0F}" name="Test Case Input" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{C8A349CF-C07B-44C4-B8D0-DD604B478305}" name="Test Oracle" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F10" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F10" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B2:F10" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7EE5C09C-96A5-4FC0-A9B8-78BA2D61269E}" name="Number" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B9AA6030-119E-443A-BB87-750EA97ECF8C}" name="Production Code Class.Method" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{49E194BC-903C-4C2D-AF6F-5DBC479ACEC9}" name="Test Code Class.Method" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{9D11DD5C-4AE4-4A5E-8750-0E12B5A106FA}" name="Test Input" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{8C3EBF53-C850-403C-B499-DB556E2F1A8B}" name="Expected Result" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7EE5C09C-96A5-4FC0-A9B8-78BA2D61269E}" name="Number" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{B9AA6030-119E-443A-BB87-750EA97ECF8C}" name="Production Code Class.Method" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{49E194BC-903C-4C2D-AF6F-5DBC479ACEC9}" name="Test Code Class.Method" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{9D11DD5C-4AE4-4A5E-8750-0E12B5A106FA}" name="Test Input" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{8C3EBF53-C850-403C-B499-DB556E2F1A8B}" name="Expected Result" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}" name="Table4" displayName="Table4" ref="A1:L513" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}" name="Table4" displayName="Table4" ref="A1:L513" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L513" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{4EEA4C52-25A8-4AC1-AB64-130F1061C5C0}" name="Control Name" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{528C3ED4-7A70-4ADC-A6E5-12A55306EB86}" name="Control A" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{5A820990-15C8-451A-AA81-A4FDEEF27F37}" name="Control B" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{90491295-6B5C-44D5-9DBA-7086E88AC0F9}" name="Control C" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{1C3B15D1-EB06-4A22-B868-6BE0E2AA4E0D}" name="Control D" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{EB1C9048-B008-4402-8AFC-D23757742E6F}" name="In Replay" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{B62C2260-705C-4FA8-AAD7-D8CDD79F071C}" name="In Game" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{7DBAE433-F5CB-4355-AA42-DF22721518A4}" name="Is Red Turn" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{E7051258-A7C3-4770-BF85-6A7E897040FA}" name="Is Blue Computer" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{672057EC-F845-40E7-A956-72F68FFFCD00}" name="Is Red Computer" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{43FEA681-4DBD-4D98-B67C-A034045E34F1}" name="Is Accessible" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{72EB1685-1373-450C-B014-35BFBA34CCA1}" name="Notes" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{4EEA4C52-25A8-4AC1-AB64-130F1061C5C0}" name="Control Name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{528C3ED4-7A70-4ADC-A6E5-12A55306EB86}" name="Control A" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{5A820990-15C8-451A-AA81-A4FDEEF27F37}" name="Control B" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{90491295-6B5C-44D5-9DBA-7086E88AC0F9}" name="Control C" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{1C3B15D1-EB06-4A22-B868-6BE0E2AA4E0D}" name="Control D" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{EB1C9048-B008-4402-8AFC-D23757742E6F}" name="In Replay" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{B62C2260-705C-4FA8-AAD7-D8CDD79F071C}" name="In Game" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{7DBAE433-F5CB-4355-AA42-DF22721518A4}" name="Is Red Turn" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{E7051258-A7C3-4770-BF85-6A7E897040FA}" name="Is Blue Computer" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{672057EC-F845-40E7-A956-72F68FFFCD00}" name="Is Red Computer" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{43FEA681-4DBD-4D98-B67C-A034045E34F1}" name="Is Accessible" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{72EB1685-1373-450C-B014-35BFBA34CCA1}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1991,15 +1991,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -2847,130 +2847,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="10.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.7109375" style="11" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.7109375" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="10">
-        <v>1</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="9" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="C6" s="11"/>
-      <c r="D6" s="11">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
         <v>1.2</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="9" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="C7" s="11"/>
-      <c r="D7" s="11">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9">
         <v>1.3</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C8" s="11"/>
-      <c r="D8" s="11">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9">
         <v>1.4</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="9" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2987,16 +2987,16 @@
       <c r="E9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3009,16 +3009,16 @@
       <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="9" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3031,16 +3031,16 @@
       <c r="E11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="9" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3053,16 +3053,16 @@
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="9" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3079,16 +3079,16 @@
       <c r="E13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="9" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3101,16 +3101,16 @@
       <c r="E14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="9" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3127,16 +3127,16 @@
       <c r="E15" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="9" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3149,16 +3149,16 @@
       <c r="E16" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="9" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3171,16 +3171,16 @@
       <c r="E17" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="9" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3193,16 +3193,16 @@
       <c r="E18" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="9" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3213,16 +3213,16 @@
       <c r="E19" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="9" t="s">
         <v>247</v>
       </c>
     </row>
@@ -3239,16 +3239,16 @@
       <c r="E20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="9" t="s">
         <v>250</v>
       </c>
     </row>
@@ -3261,16 +3261,16 @@
       <c r="E21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="9" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3283,37 +3283,37 @@
       <c r="E22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="9" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="C23" s="11"/>
-      <c r="D23" s="11">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
         <v>8.4</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="9" t="s">
         <v>257</v>
       </c>
     </row>
@@ -3335,122 +3335,122 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="11"/>
-    <col min="2" max="2" width="15" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.7109375" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.7109375" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>1.2</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="9" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>1.3</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>1.4</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="9" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="9" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3467,13 +3467,13 @@
       <c r="E9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3486,13 +3486,13 @@
       <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3505,13 +3505,13 @@
       <c r="E11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="9" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3524,24 +3524,24 @@
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="9" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="9" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3558,13 +3558,13 @@
       <c r="E14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="9" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3577,13 +3577,13 @@
       <c r="E15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="9" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3600,13 +3600,13 @@
       <c r="E16" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="9" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3619,13 +3619,13 @@
       <c r="E17" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="9" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3638,13 +3638,13 @@
       <c r="E18" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="9" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3657,13 +3657,13 @@
       <c r="E19" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="9" t="s">
         <v>245</v>
       </c>
     </row>
@@ -3676,13 +3676,13 @@
       <c r="E20" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="9" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3699,13 +3699,13 @@
       <c r="E21" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3718,13 +3718,13 @@
       <c r="E22" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="9" t="s">
         <v>262</v>
       </c>
     </row>
@@ -3737,24 +3737,24 @@
       <c r="E23" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>8.4</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="9" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3770,105 +3770,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF00AFE-AD52-4AB4-8B4B-3CE4DDE5BDEE}">
   <dimension ref="B3:G19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="39.85546875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="38.7109375" style="10" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="38.7109375" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9">
         <v>1.2</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="11"/>
-      <c r="D6" s="11">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
         <v>1.3</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C7" s="11"/>
-      <c r="D7" s="11">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9">
         <v>1.4</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3885,10 +3885,10 @@
       <c r="E8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="9" t="s">
         <v>270</v>
       </c>
     </row>
@@ -3901,10 +3901,10 @@
       <c r="E9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="9" t="s">
         <v>272</v>
       </c>
     </row>
@@ -3917,10 +3917,10 @@
       <c r="E10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="9" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3937,10 +3937,10 @@
       <c r="E11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3953,10 +3953,10 @@
       <c r="E12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="9" t="s">
         <v>278</v>
       </c>
     </row>
@@ -3973,10 +3973,10 @@
       <c r="E13" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="9" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3989,10 +3989,10 @@
       <c r="E14" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="9" t="s">
         <v>282</v>
       </c>
     </row>
@@ -4005,10 +4005,10 @@
       <c r="E15" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="9" t="s">
         <v>284</v>
       </c>
     </row>
@@ -4021,10 +4021,10 @@
       <c r="E16" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>287</v>
       </c>
     </row>
@@ -4041,10 +4041,10 @@
       <c r="E17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="9" t="s">
         <v>289</v>
       </c>
     </row>
@@ -4057,26 +4057,26 @@
       <c r="E18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="9" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9">
         <v>8.4</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="9" t="s">
         <v>293</v>
       </c>
     </row>
@@ -4092,172 +4092,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16732A8-5A44-436B-B9F8-A4670902CDC5}">
   <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="11"/>
-    <col min="2" max="2" width="10.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" style="11" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="10.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="11">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="F3" s="11" t="b">
+      <c r="F3" s="9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F4" s="11" t="b">
+      <c r="F4" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="F5" s="11" t="b">
+      <c r="F5" s="9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F6" s="11" t="b">
+      <c r="F6" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>7</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="9" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="F10" s="11" t="b">
+      <c r="F10" s="9" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>